<commit_message>
Added collagen and skin examples
</commit_message>
<xml_diff>
--- a/examples/ecm_proteins.xlsx
+++ b/examples/ecm_proteins.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>N_content</t>
   </si>
@@ -43,9 +43,6 @@
     <t>col3_a1_hum_uniprot</t>
   </si>
   <si>
-    <t>col3_hum_chung_1974</t>
-  </si>
-  <si>
     <t>col4_a1_hum_uniprot</t>
   </si>
   <si>
@@ -173,6 +170,24 @@
   </si>
   <si>
     <t>laminin-523_hum_uniprot</t>
+  </si>
+  <si>
+    <t>Collagen_1_hum_uitto_1978</t>
+  </si>
+  <si>
+    <t>Collagen_3_hum_chung_1974</t>
+  </si>
+  <si>
+    <t>Collagen_4_hum_glanville_1979</t>
+  </si>
+  <si>
+    <t>Skin-Collagen_hum_bornstein_1964</t>
+  </si>
+  <si>
+    <t>Skin-Collagen_hum_acid_miyahara_1978</t>
+  </si>
+  <si>
+    <t>Skin-Collagen_hum_age0_miyahara_1978</t>
   </si>
 </sst>
 </file>
@@ -530,7 +545,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -630,19 +645,22 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.1826407971543893</v>
+        <v>0.1757517677829037</v>
       </c>
       <c r="C5">
-        <v>5.475227964290386</v>
+        <v>5.689843195405262</v>
+      </c>
+      <c r="D5">
+        <v>144249.6273</v>
       </c>
       <c r="E5">
-        <v>0.1555862244343698</v>
+        <v>0.01176234928130036</v>
       </c>
       <c r="F5">
-        <v>0.1803669007380068</v>
+        <v>0.01363577330177446</v>
       </c>
       <c r="G5">
-        <v>1.375481588789803</v>
+        <v>0.1039866796444327</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -650,22 +668,22 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.1757517677829037</v>
+        <v>0.1789502314631272</v>
       </c>
       <c r="C6">
-        <v>5.689843195405262</v>
+        <v>5.588145887400267</v>
       </c>
       <c r="D6">
-        <v>144249.6273</v>
+        <v>149185.4466</v>
       </c>
       <c r="E6">
-        <v>0.01176234928130036</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0.01363577330177446</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>0.1039866796444327</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -673,13 +691,13 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>0.1789502314631272</v>
+        <v>0.1796502121333101</v>
       </c>
       <c r="C7">
-        <v>5.588145887400267</v>
+        <v>5.566372497561797</v>
       </c>
       <c r="D7">
-        <v>149185.4466</v>
+        <v>158973.7132</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -696,13 +714,13 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>0.1796502121333101</v>
+        <v>0.1817286195715312</v>
       </c>
       <c r="C8">
-        <v>5.566372497561797</v>
+        <v>5.502710593178664</v>
       </c>
       <c r="D8">
-        <v>158973.7132</v>
+        <v>159621.9449</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -719,13 +737,13 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>0.1817286195715312</v>
+        <v>0.176459814086915</v>
       </c>
       <c r="C9">
-        <v>5.502710593178664</v>
+        <v>5.667012657666359</v>
       </c>
       <c r="D9">
-        <v>159621.9449</v>
+        <v>159466.6777</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -742,13 +760,13 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>0.176459814086915</v>
+        <v>0.1767436010476583</v>
       </c>
       <c r="C10">
-        <v>5.667012657666359</v>
+        <v>5.657913463754499</v>
       </c>
       <c r="D10">
-        <v>159466.6777</v>
+        <v>161350.3461</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -765,22 +783,22 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>0.1767436010476583</v>
+        <v>0.1884189740769391</v>
       </c>
       <c r="C11">
-        <v>5.657913463754499</v>
+        <v>5.307321117201603</v>
       </c>
       <c r="D11">
-        <v>161350.3461</v>
+        <v>96639.4711</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.129922972022557</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>0.1506161865137639</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1.148602047691329</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -788,22 +806,22 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>0.1884189740769391</v>
+        <v>0.1855787998593464</v>
       </c>
       <c r="C12">
-        <v>5.307321117201603</v>
+        <v>5.38854654064968</v>
       </c>
       <c r="D12">
-        <v>96639.4711</v>
+        <v>124987.85</v>
       </c>
       <c r="E12">
-        <v>0.129922972022557</v>
+        <v>0.06606517273478983</v>
       </c>
       <c r="F12">
-        <v>0.1506161865137639</v>
+        <v>0.07658756741617298</v>
       </c>
       <c r="G12">
-        <v>1.148602047691329</v>
+        <v>0.5840583193485318</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -811,22 +829,22 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>0.1855787998593464</v>
+        <v>0.1937549794010582</v>
       </c>
       <c r="C13">
-        <v>5.38854654064968</v>
+        <v>5.161157680134123</v>
       </c>
       <c r="D13">
-        <v>124987.85</v>
+        <v>93761.15109999999</v>
       </c>
       <c r="E13">
-        <v>0.06606517273478983</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>0.07658756741617298</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>0.5840583193485318</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -834,22 +852,22 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>0.1937549794010582</v>
+        <v>0.1768522902144926</v>
       </c>
       <c r="C14">
-        <v>5.161157680134123</v>
+        <v>5.654436246130402</v>
       </c>
       <c r="D14">
-        <v>93761.15109999999</v>
+        <v>157766.3844</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>0.01075460090216785</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>0.01246751786959413</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>0.09507754037668062</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -857,22 +875,22 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>0.1768522902144926</v>
+        <v>0.1654405831065965</v>
       </c>
       <c r="C15">
-        <v>5.654436246130402</v>
+        <v>6.044466123258771</v>
       </c>
       <c r="D15">
-        <v>157766.3844</v>
+        <v>25060.255</v>
       </c>
       <c r="E15">
-        <v>0.01075460090216785</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>0.01246751786959413</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>0.09507754037668062</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -880,22 +898,22 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.1654405831065965</v>
+        <v>0.1726705521778199</v>
       </c>
       <c r="C16">
-        <v>6.044466123258771</v>
+        <v>5.791375468413273</v>
       </c>
       <c r="D16">
-        <v>25060.255</v>
+        <v>47616.3005</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>0.004751074687123163</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>0.005507792348625814</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>0.04200253449726084</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -903,22 +921,22 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.1726705521778199</v>
+        <v>0.1769561022098064</v>
       </c>
       <c r="C17">
-        <v>5.791375468413273</v>
+        <v>5.651119048804312</v>
       </c>
       <c r="D17">
-        <v>47616.3005</v>
+        <v>46383.96809999999</v>
       </c>
       <c r="E17">
-        <v>0.004751074687123163</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>0.005507792348625814</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>0.04200253449726084</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -926,13 +944,13 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>0.1769561022098064</v>
+        <v>0.170158201328237</v>
       </c>
       <c r="C18">
-        <v>5.651119048804312</v>
+        <v>5.87688393620822</v>
       </c>
       <c r="D18">
-        <v>46383.96809999999</v>
+        <v>269254.819</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -949,13 +967,13 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>0.170158201328237</v>
+        <v>0.1740090842433178</v>
       </c>
       <c r="C19">
-        <v>5.87688393620822</v>
+        <v>5.746826404773757</v>
       </c>
       <c r="D19">
-        <v>269254.819</v>
+        <v>335338.3098</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -972,13 +990,13 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.1740090842433178</v>
+        <v>0.1726710561980939</v>
       </c>
       <c r="C20">
-        <v>5.746826404773757</v>
+        <v>5.791358563607598</v>
       </c>
       <c r="D20">
-        <v>335338.3098</v>
+        <v>341911.6196999999</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -995,13 +1013,13 @@
         <v>25</v>
       </c>
       <c r="B21">
-        <v>0.1726710561980939</v>
+        <v>0.1763908190353961</v>
       </c>
       <c r="C21">
-        <v>5.791358563607598</v>
+        <v>5.669229302684577</v>
       </c>
       <c r="D21">
-        <v>341911.6196999999</v>
+        <v>363129.0985</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1018,13 +1036,13 @@
         <v>26</v>
       </c>
       <c r="B22">
-        <v>0.1763908190353961</v>
+        <v>0.1727506988998854</v>
       </c>
       <c r="C22">
-        <v>5.669229302684577</v>
+        <v>5.788688592105392</v>
       </c>
       <c r="D22">
-        <v>363129.0985</v>
+        <v>199863.2464</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1041,13 +1059,13 @@
         <v>27</v>
       </c>
       <c r="B23">
-        <v>0.1727506988998854</v>
+        <v>0.1803207130723951</v>
       </c>
       <c r="C23">
-        <v>5.788688592105392</v>
+        <v>5.545674609208763</v>
       </c>
       <c r="D23">
-        <v>199863.2464</v>
+        <v>396306.0159999999</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1064,13 +1082,13 @@
         <v>28</v>
       </c>
       <c r="B24">
-        <v>0.1803207130723951</v>
+        <v>0.1692648711370833</v>
       </c>
       <c r="C24">
-        <v>5.545674609208763</v>
+        <v>5.907900400610152</v>
       </c>
       <c r="D24">
-        <v>396306.0159999999</v>
+        <v>195704.1959</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1087,13 +1105,13 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>0.1692648711370833</v>
+        <v>0.1855200624810122</v>
       </c>
       <c r="C25">
-        <v>5.907900400610152</v>
+        <v>5.390252604633252</v>
       </c>
       <c r="D25">
-        <v>195704.1959</v>
+        <v>192448.6108</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1110,13 +1128,13 @@
         <v>30</v>
       </c>
       <c r="B26">
-        <v>0.1855200624810122</v>
+        <v>0.1843527561098423</v>
       </c>
       <c r="C26">
-        <v>5.390252604633252</v>
+        <v>5.424383237341857</v>
       </c>
       <c r="D26">
-        <v>192448.6108</v>
+        <v>127642.5506</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1133,13 +1151,13 @@
         <v>31</v>
       </c>
       <c r="B27">
-        <v>0.1843527561098423</v>
+        <v>0.1744889847369807</v>
       </c>
       <c r="C27">
-        <v>5.424383237341857</v>
+        <v>5.731020794850571</v>
       </c>
       <c r="D27">
-        <v>127642.5506</v>
+        <v>193537.4531</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1156,13 +1174,13 @@
         <v>32</v>
       </c>
       <c r="B28">
-        <v>0.1744889847369807</v>
+        <v>0.1740793325444005</v>
       </c>
       <c r="C28">
-        <v>5.731020794850571</v>
+        <v>5.74450731964371</v>
       </c>
       <c r="D28">
-        <v>193537.4531</v>
+        <v>174279.8054</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1179,13 +1197,13 @@
         <v>33</v>
       </c>
       <c r="B29">
-        <v>0.1740793325444005</v>
+        <v>0.1803841954275984</v>
       </c>
       <c r="C29">
-        <v>5.74450731964371</v>
+        <v>5.54372292777376</v>
       </c>
       <c r="D29">
-        <v>174279.8054</v>
+        <v>128742.4796</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -1202,13 +1220,13 @@
         <v>34</v>
       </c>
       <c r="B30">
-        <v>0.1803841954275984</v>
+        <v>0.180084606122577</v>
       </c>
       <c r="C30">
-        <v>5.54372292777376</v>
+        <v>5.552945482299228</v>
       </c>
       <c r="D30">
-        <v>128742.4796</v>
+        <v>169479.224</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1225,22 +1243,22 @@
         <v>35</v>
       </c>
       <c r="B31">
-        <v>0.180084606122577</v>
+        <v>0.1906055886291117</v>
       </c>
       <c r="C31">
-        <v>5.552945482299228</v>
+        <v>5.246435884657305</v>
       </c>
       <c r="D31">
-        <v>169479.224</v>
+        <v>287180.3707</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>0.08941051937990274</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>0.103651196193987</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>0.790446093144109</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1248,22 +1266,22 @@
         <v>36</v>
       </c>
       <c r="B32">
-        <v>0.1906055886291117</v>
+        <v>0.1873035976764402</v>
       </c>
       <c r="C32">
-        <v>5.246435884657305</v>
+        <v>5.338925746250008</v>
       </c>
       <c r="D32">
-        <v>287180.3707</v>
+        <v>318266.7922</v>
       </c>
       <c r="E32">
-        <v>0.08941051937990274</v>
+        <v>0.1048451152234286</v>
       </c>
       <c r="F32">
-        <v>0.103651196193987</v>
+        <v>0.1215441055859415</v>
       </c>
       <c r="G32">
-        <v>0.790446093144109</v>
+        <v>0.9268977776705677</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1271,22 +1289,22 @@
         <v>37</v>
       </c>
       <c r="B33">
-        <v>0.1873035976764402</v>
+        <v>0.1727100759226217</v>
       </c>
       <c r="C33">
-        <v>5.338925746250008</v>
+        <v>5.790050144196706</v>
       </c>
       <c r="D33">
-        <v>318266.7922</v>
+        <v>705322.3110999999</v>
       </c>
       <c r="E33">
-        <v>0.1048451152234286</v>
+        <v>0</v>
       </c>
       <c r="F33">
-        <v>0.1215441055859415</v>
+        <v>0</v>
       </c>
       <c r="G33">
-        <v>0.9268977776705677</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1294,13 +1312,13 @@
         <v>38</v>
       </c>
       <c r="B34">
-        <v>0.1727100759226217</v>
+        <v>0.1720794377522938</v>
       </c>
       <c r="C34">
-        <v>5.790050144196706</v>
+        <v>5.811269568648217</v>
       </c>
       <c r="D34">
-        <v>705322.3110999999</v>
+        <v>711895.6209999998</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1317,13 +1335,13 @@
         <v>39</v>
       </c>
       <c r="B35">
-        <v>0.1720794377522938</v>
+        <v>0.1771818804299807</v>
       </c>
       <c r="C35">
-        <v>5.811269568648217</v>
+        <v>5.643917976111464</v>
       </c>
       <c r="D35">
-        <v>711895.6209999998</v>
+        <v>702066.7259999999</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -1340,13 +1358,13 @@
         <v>40</v>
       </c>
       <c r="B36">
-        <v>0.1771818804299807</v>
+        <v>0.1765068647880498</v>
       </c>
       <c r="C36">
-        <v>5.643917976111464</v>
+        <v>5.665502025662313</v>
       </c>
       <c r="D36">
-        <v>702066.7259999999</v>
+        <v>708640.0358999998</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -1363,13 +1381,13 @@
         <v>41</v>
       </c>
       <c r="B37">
-        <v>0.1765068647880498</v>
+        <v>0.1788611406369691</v>
       </c>
       <c r="C37">
-        <v>5.665502025662313</v>
+        <v>5.590929345741344</v>
       </c>
       <c r="D37">
-        <v>708640.0358999998</v>
+        <v>619514.1286999999</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -1386,13 +1404,13 @@
         <v>42</v>
       </c>
       <c r="B38">
-        <v>0.1788611406369691</v>
+        <v>0.1739390509251408</v>
       </c>
       <c r="C38">
-        <v>5.590929345741344</v>
+        <v>5.749140257355872</v>
       </c>
       <c r="D38">
-        <v>619514.1286999999</v>
+        <v>733113.0998</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -1409,13 +1427,13 @@
         <v>43</v>
       </c>
       <c r="B39">
-        <v>0.1739390509251408</v>
+        <v>0.1782460644437892</v>
       </c>
       <c r="C39">
-        <v>5.749140257355872</v>
+        <v>5.610222044006783</v>
       </c>
       <c r="D39">
-        <v>733113.0998</v>
+        <v>729857.5146999999</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -1432,13 +1450,13 @@
         <v>44</v>
       </c>
       <c r="B40">
-        <v>0.1782460644437892</v>
+        <v>0.1719598955606222</v>
       </c>
       <c r="C40">
-        <v>5.610222044006783</v>
+        <v>5.815309416999868</v>
       </c>
       <c r="D40">
-        <v>729857.5146999999</v>
+        <v>569847.2476999999</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -1455,13 +1473,13 @@
         <v>45</v>
       </c>
       <c r="B41">
-        <v>0.1719598955606222</v>
+        <v>0.1774966217090255</v>
       </c>
       <c r="C41">
-        <v>5.815309416999868</v>
+        <v>5.633910044999753</v>
       </c>
       <c r="D41">
-        <v>569847.2476999999</v>
+        <v>566591.6625999999</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -1478,13 +1496,13 @@
         <v>46</v>
       </c>
       <c r="B42">
-        <v>0.1774966217090255</v>
+        <v>0.1760776443041887</v>
       </c>
       <c r="C42">
-        <v>5.633910044999753</v>
+        <v>5.679312691578366</v>
       </c>
       <c r="D42">
-        <v>566591.6625999999</v>
+        <v>766290.0172999999</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -1501,13 +1519,13 @@
         <v>47</v>
       </c>
       <c r="B43">
-        <v>0.1760776443041887</v>
+        <v>0.1802065124421</v>
       </c>
       <c r="C43">
-        <v>5.679312691578366</v>
+        <v>5.549189019022262</v>
       </c>
       <c r="D43">
-        <v>766290.0172999999</v>
+        <v>763034.4321999999</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -1524,13 +1542,13 @@
         <v>48</v>
       </c>
       <c r="B44">
-        <v>0.1802065124421</v>
+        <v>0.1753682050985928</v>
       </c>
       <c r="C44">
-        <v>5.549189019022262</v>
+        <v>5.702287934336759</v>
       </c>
       <c r="D44">
-        <v>763034.4321999999</v>
+        <v>643833.9756999998</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -1547,13 +1565,13 @@
         <v>49</v>
       </c>
       <c r="B45">
-        <v>0.1753682050985928</v>
+        <v>0.179677361482587</v>
       </c>
       <c r="C45">
-        <v>5.702287934336759</v>
+        <v>5.565531415580771</v>
       </c>
       <c r="D45">
-        <v>643833.9756999998</v>
+        <v>725056.9332999999</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -1570,13 +1588,13 @@
         <v>50</v>
       </c>
       <c r="B46">
-        <v>0.179677361482587</v>
+        <v>0.1793374734337096</v>
       </c>
       <c r="C46">
-        <v>5.565531415580771</v>
+        <v>5.576079448725145</v>
       </c>
       <c r="D46">
-        <v>725056.9332999999</v>
+        <v>561791.0811999999</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -1593,13 +1611,13 @@
         <v>51</v>
       </c>
       <c r="B47">
-        <v>0.1793374734337096</v>
+        <v>0.1815875944535185</v>
       </c>
       <c r="C47">
-        <v>5.576079448725145</v>
+        <v>5.506984125261779</v>
       </c>
       <c r="D47">
-        <v>561791.0811999999</v>
+        <v>758233.8507999999</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -1616,22 +1634,119 @@
         <v>52</v>
       </c>
       <c r="B48">
-        <v>0.1815875944535185</v>
+        <v>0.1843275692130446</v>
       </c>
       <c r="C48">
-        <v>5.506984125261779</v>
-      </c>
-      <c r="D48">
-        <v>758233.8507999999</v>
+        <v>5.425124436183536</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>0.1169947657113922</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>0.1356288666985065</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>1.034308447330943</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49">
+        <v>0.1826407971543893</v>
+      </c>
+      <c r="C49">
+        <v>5.475227964290386</v>
+      </c>
+      <c r="E49">
+        <v>0.1555862244343698</v>
+      </c>
+      <c r="F49">
+        <v>0.1803669007380068</v>
+      </c>
+      <c r="G49">
+        <v>1.375481588789803</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50">
+        <v>0.1643559632507289</v>
+      </c>
+      <c r="C50">
+        <v>6.084354837034276</v>
+      </c>
+      <c r="E50">
+        <v>0.1695406238034565</v>
+      </c>
+      <c r="F50">
+        <v>0.1965438584025607</v>
+      </c>
+      <c r="G50">
+        <v>1.498847391158093</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51">
+        <v>0.1833505892952129</v>
+      </c>
+      <c r="C51">
+        <v>5.454032102345193</v>
+      </c>
+      <c r="E51">
+        <v>0.116479586664021</v>
+      </c>
+      <c r="F51">
+        <v>0.135031633566606</v>
+      </c>
+      <c r="G51">
+        <v>1.029753935534248</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52">
+        <v>0.183701390849173</v>
+      </c>
+      <c r="C52">
+        <v>5.443616922971718</v>
+      </c>
+      <c r="E52">
+        <v>0.114902561622547</v>
+      </c>
+      <c r="F52">
+        <v>0.1332034311010537</v>
+      </c>
+      <c r="G52">
+        <v>1.015812027004146</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53">
+        <v>0.1798439066934646</v>
+      </c>
+      <c r="C53">
+        <v>5.560377431660513</v>
+      </c>
+      <c r="E53">
+        <v>0.1148732530857138</v>
+      </c>
+      <c r="F53">
+        <v>0.1331694545072196</v>
+      </c>
+      <c r="G53">
+        <v>1.01555292082071</v>
       </c>
     </row>
   </sheetData>

</xml_diff>